<commit_message>
Auto commit on 2025/05/27 週二 20:46:39.05
</commit_message>
<xml_diff>
--- a/IM/202505_HL_Maintain_Report.xlsx
+++ b/IM/202505_HL_Maintain_Report.xlsx
@@ -11,14 +11,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$140</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$141</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="953">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="961">
   <si>
     <t>萊爾富 工作統計表  篩選月份：202505   (  製表日期:2025-05-27  )</t>
   </si>
@@ -2955,6 +2955,31 @@
   </si>
   <si>
     <t>2025-05-27 13:39:00</t>
+  </si>
+  <si>
+    <t>14101114052701</t>
+  </si>
+  <si>
+    <t>2025-05-27 16:48:47</t>
+  </si>
+  <si>
+    <t>2025/05/27 緊急叫修：門市SC(SHUTTLE6S)開啟HISHOP、訂貨3.0、E網…任何一支程式，出現訊息「參照的磁碟機或網路連線無法使用，請確認插入的磁碟正確，而且網路資源可以使用，然後重試。」因開啟HISHOP、訂貨3.0、E網…任何一支程式都出現異常訊息，請更換第二顆硬碟不備份還原，並攜帶主機隨行檢測........還請台芝協助</t>
+  </si>
+  <si>
+    <t>2025-05-27 16:54:25</t>
+  </si>
+  <si>
+    <t>2025-05-27 17:50:00</t>
+  </si>
+  <si>
+    <t>2025-05-27 18:50:00</t>
+  </si>
+  <si>
+    <t>2025-05-28 09:54:00</t>
+  </si>
+  <si>
+    <t>更換硬碟排線（無更換硬碟）
+已請0800測試正常</t>
   </si>
 </sst>
 </file>
@@ -3368,10 +3393,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK140"/>
+  <dimension ref="A1:AK141"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="AC137" sqref="AC137"/>
+      <selection activeCell="A141" sqref="A141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15378,7 +15403,7 @@
       <c r="M140" s="4"/>
       <c r="N140" s="3"/>
       <c r="O140" s="4"/>
-      <c r="P140" s="4"/>
+      <c r="P140" s="10"/>
       <c r="Q140" s="3" t="s">
         <v>950</v>
       </c>
@@ -15411,7 +15436,7 @@
       <c r="AB140" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="AC140" s="4" t="s">
+      <c r="AC140" s="10" t="s">
         <v>152</v>
       </c>
       <c r="AD140" s="3" t="s">
@@ -15426,6 +15451,103 @@
         <v>61</v>
       </c>
       <c r="AK140" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="141" spans="1:37">
+      <c r="A141" s="7">
+        <v>139</v>
+      </c>
+      <c r="B141" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C141" s="7">
+        <v>2025053506</v>
+      </c>
+      <c r="D141" s="7" t="s">
+        <v>953</v>
+      </c>
+      <c r="E141" s="7" t="s">
+        <v>459</v>
+      </c>
+      <c r="F141" s="7">
+        <v>4101</v>
+      </c>
+      <c r="G141" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="H141" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="I141" s="7" t="s">
+        <v>954</v>
+      </c>
+      <c r="J141" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="K141" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L141" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="M141" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="N141" s="7">
+        <v>2405</v>
+      </c>
+      <c r="O141" s="8" t="s">
+        <v>541</v>
+      </c>
+      <c r="P141" s="8" t="s">
+        <v>955</v>
+      </c>
+      <c r="Q141" s="7" t="s">
+        <v>364</v>
+      </c>
+      <c r="R141" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S141" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="T141" s="7">
+        <v>1</v>
+      </c>
+      <c r="U141" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V141" s="7" t="s">
+        <v>956</v>
+      </c>
+      <c r="W141" s="7" t="s">
+        <v>957</v>
+      </c>
+      <c r="X141" s="7" t="s">
+        <v>958</v>
+      </c>
+      <c r="Y141" s="7" t="s">
+        <v>959</v>
+      </c>
+      <c r="Z141" s="7">
+        <v>1</v>
+      </c>
+      <c r="AA141" s="7"/>
+      <c r="AB141" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC141" s="8" t="s">
+        <v>960</v>
+      </c>
+      <c r="AD141" s="7"/>
+      <c r="AE141" s="7"/>
+      <c r="AF141" s="7"/>
+      <c r="AG141" s="7"/>
+      <c r="AH141" s="7"/>
+      <c r="AI141" s="7"/>
+      <c r="AJ141" s="7"/>
+      <c r="AK141" s="7" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit on 2025/05/28 週三 14:47:13.05
</commit_message>
<xml_diff>
--- a/IM/202505_HL_Maintain_Report.xlsx
+++ b/IM/202505_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$141</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$145</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="961">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202505   (  製表日期:2025-05-27  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="984">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202505   (  製表日期:2025-05-28  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -2909,6 +2909,33 @@
     <t>更換鍵盤</t>
   </si>
   <si>
+    <t>15352114052701</t>
+  </si>
+  <si>
+    <t>2025-05-27 11:15:30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">總公司健誌副理叫修sc(SHUTTLE6S):Computer: H5352  Description: 已重試磁碟 1 (PDO 名稱: \\Device\\00000035) 邏輯區塊位址 0x1703337 上的 IO 操作。此狀況造成銷售引擎無法依時運作，且可能發生TM轉SC的問題。請到店更換門市SC第二顆硬碟，資料不要備份。與門市確認今日訂貨3.0正常，hishop目前可正常開啟...請台芝到店協助
+PS.若因更換HD.請跟店長宣達:1.請門市先回報代收會計 2.請確認SC的代收資料是否正確 (須與代收單據逐一核對)																																
+與門市確認帳務做到05/26，與通訊功評確認有收到05/26的銷售																																
+</t>
+  </si>
+  <si>
+    <t>2025-05-27 11:52:05</t>
+  </si>
+  <si>
+    <t>2025-05-27 18:20:00</t>
+  </si>
+  <si>
+    <t>2025-05-27 20:56:00</t>
+  </si>
+  <si>
+    <t>2025-05-28 15:52:00</t>
+  </si>
+  <si>
+    <t>更換第二顆硬碟不備份還原完成</t>
+  </si>
+  <si>
     <t>12209114052701</t>
   </si>
   <si>
@@ -2980,6 +3007,51 @@
   <si>
     <t>更換硬碟排線（無更換硬碟）
 已請0800測試正常</t>
+  </si>
+  <si>
+    <t>14834114052703</t>
+  </si>
+  <si>
+    <t>2025-05-27 18:40:47</t>
+  </si>
+  <si>
+    <t>門市TM1多卡機(QP3000E)悠遊卡跟一卡通皆無法使用,已有協助版更並將悠遊卡重開，但TM顯示通訊逾時，將一卡通重開顯示0801 錯誤訊息.......還請台芝到店協助</t>
+  </si>
+  <si>
+    <t>2025-05-27 18:50:39</t>
+  </si>
+  <si>
+    <t>2025-05-28 10:30:00</t>
+  </si>
+  <si>
+    <t>2025-05-28 10:50:00</t>
+  </si>
+  <si>
+    <t>2025-05-28 22:50:00</t>
+  </si>
+  <si>
+    <t>重接排線手動版本更新 測試正常</t>
+  </si>
+  <si>
+    <t>林口香澄店</t>
+  </si>
+  <si>
+    <t>THILF04057</t>
+  </si>
+  <si>
+    <t>2025-05-28 13:55:40</t>
+  </si>
+  <si>
+    <t>2025-05-28 13:00:00</t>
+  </si>
+  <si>
+    <t>2025-05-28 14:00:00</t>
+  </si>
+  <si>
+    <t>2025-05-28 14:20:29</t>
+  </si>
+  <si>
+    <t>2025-05-28 14:10:00</t>
   </si>
 </sst>
 </file>
@@ -3393,10 +3465,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK141"/>
+  <dimension ref="A1:AK145"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A141" sqref="A141"/>
+      <selection activeCell="A145" sqref="A145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15128,7 +15200,7 @@
         <v>38</v>
       </c>
       <c r="C137" s="7">
-        <v>2025053434</v>
+        <v>2025053432</v>
       </c>
       <c r="D137" s="7" t="s">
         <v>937</v>
@@ -15137,10 +15209,10 @@
         <v>40</v>
       </c>
       <c r="F137" s="7">
-        <v>2209</v>
+        <v>5352</v>
       </c>
       <c r="G137" s="7" t="s">
-        <v>337</v>
+        <v>800</v>
       </c>
       <c r="H137" s="7" t="s">
         <v>86</v>
@@ -15152,25 +15224,25 @@
         <v>274</v>
       </c>
       <c r="K137" s="7" t="s">
-        <v>45</v>
+        <v>100</v>
       </c>
       <c r="L137" s="7" t="s">
-        <v>275</v>
+        <v>244</v>
       </c>
       <c r="M137" s="8" t="s">
-        <v>276</v>
-      </c>
-      <c r="N137" s="7" t="s">
-        <v>606</v>
+        <v>245</v>
+      </c>
+      <c r="N137" s="7">
+        <v>2405</v>
       </c>
       <c r="O137" s="8" t="s">
-        <v>158</v>
+        <v>541</v>
       </c>
       <c r="P137" s="9" t="s">
         <v>939</v>
       </c>
       <c r="Q137" s="7" t="s">
-        <v>340</v>
+        <v>803</v>
       </c>
       <c r="R137" s="7" t="s">
         <v>52</v>
@@ -15197,7 +15269,7 @@
         <v>943</v>
       </c>
       <c r="Z137" s="7">
-        <v>0.5</v>
+        <v>2.6</v>
       </c>
       <c r="AA137" s="7"/>
       <c r="AB137" s="7" t="s">
@@ -15222,38 +15294,58 @@
         <v>136</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>132</v>
+        <v>38</v>
       </c>
       <c r="C138" s="3">
-        <v>2025053435</v>
-      </c>
-      <c r="D138" s="3"/>
-      <c r="E138" s="3"/>
+        <v>2025053434</v>
+      </c>
+      <c r="D138" s="3" t="s">
+        <v>945</v>
+      </c>
+      <c r="E138" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="F138" s="3">
-        <v>4538</v>
+        <v>2209</v>
       </c>
       <c r="G138" s="3" t="s">
-        <v>921</v>
+        <v>337</v>
       </c>
       <c r="H138" s="3" t="s">
-        <v>272</v>
-      </c>
-      <c r="I138" s="3"/>
-      <c r="J138" s="3"/>
-      <c r="K138" s="3"/>
-      <c r="L138" s="3"/>
-      <c r="M138" s="4"/>
-      <c r="N138" s="3"/>
-      <c r="O138" s="4"/>
-      <c r="P138" s="10"/>
+        <v>86</v>
+      </c>
+      <c r="I138" s="3" t="s">
+        <v>946</v>
+      </c>
+      <c r="J138" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="K138" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L138" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="M138" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="N138" s="3" t="s">
+        <v>606</v>
+      </c>
+      <c r="O138" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="P138" s="10" t="s">
+        <v>947</v>
+      </c>
       <c r="Q138" s="3" t="s">
-        <v>924</v>
+        <v>340</v>
       </c>
       <c r="R138" s="3" t="s">
         <v>52</v>
       </c>
       <c r="S138" s="3" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="T138" s="3">
         <v>1</v>
@@ -15262,36 +15354,34 @@
         <v>54</v>
       </c>
       <c r="V138" s="3" t="s">
-        <v>945</v>
+        <v>948</v>
       </c>
       <c r="W138" s="3" t="s">
-        <v>934</v>
+        <v>949</v>
       </c>
       <c r="X138" s="3" t="s">
-        <v>946</v>
-      </c>
-      <c r="Y138" s="3"/>
+        <v>950</v>
+      </c>
+      <c r="Y138" s="3" t="s">
+        <v>951</v>
+      </c>
       <c r="Z138" s="3">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="AA138" s="3"/>
       <c r="AB138" s="3" t="s">
         <v>59</v>
       </c>
       <c r="AC138" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="AD138" s="3" t="s">
-        <v>61</v>
-      </c>
+        <v>952</v>
+      </c>
+      <c r="AD138" s="3"/>
       <c r="AE138" s="3"/>
       <c r="AF138" s="3"/>
       <c r="AG138" s="3"/>
       <c r="AH138" s="3"/>
       <c r="AI138" s="3"/>
-      <c r="AJ138" s="3" t="s">
-        <v>61</v>
-      </c>
+      <c r="AJ138" s="3"/>
       <c r="AK138" s="3" t="s">
         <v>61</v>
       </c>
@@ -15304,18 +15394,18 @@
         <v>132</v>
       </c>
       <c r="C139" s="7">
-        <v>2025053438</v>
+        <v>2025053435</v>
       </c>
       <c r="D139" s="7"/>
       <c r="E139" s="7"/>
-      <c r="F139" s="7" t="s">
-        <v>706</v>
+      <c r="F139" s="7">
+        <v>4538</v>
       </c>
       <c r="G139" s="7" t="s">
-        <v>707</v>
+        <v>921</v>
       </c>
       <c r="H139" s="7" t="s">
-        <v>86</v>
+        <v>272</v>
       </c>
       <c r="I139" s="7"/>
       <c r="J139" s="7"/>
@@ -15326,13 +15416,13 @@
       <c r="O139" s="8"/>
       <c r="P139" s="9"/>
       <c r="Q139" s="7" t="s">
-        <v>710</v>
+        <v>924</v>
       </c>
       <c r="R139" s="7" t="s">
         <v>52</v>
       </c>
       <c r="S139" s="7" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="T139" s="7">
         <v>1</v>
@@ -15341,24 +15431,24 @@
         <v>54</v>
       </c>
       <c r="V139" s="7" t="s">
-        <v>947</v>
+        <v>953</v>
       </c>
       <c r="W139" s="7" t="s">
-        <v>857</v>
+        <v>934</v>
       </c>
       <c r="X139" s="7" t="s">
-        <v>948</v>
+        <v>954</v>
       </c>
       <c r="Y139" s="7"/>
       <c r="Z139" s="7">
-        <v>1.7</v>
+        <v>0.3</v>
       </c>
       <c r="AA139" s="7"/>
       <c r="AB139" s="7" t="s">
         <v>59</v>
       </c>
       <c r="AC139" s="9" t="s">
-        <v>152</v>
+        <v>134</v>
       </c>
       <c r="AD139" s="7" t="s">
         <v>61</v>
@@ -15383,18 +15473,18 @@
         <v>132</v>
       </c>
       <c r="C140" s="3">
-        <v>2025053457</v>
+        <v>2025053438</v>
       </c>
       <c r="D140" s="3"/>
       <c r="E140" s="3"/>
-      <c r="F140" s="3">
-        <v>3955</v>
+      <c r="F140" s="3" t="s">
+        <v>706</v>
       </c>
       <c r="G140" s="3" t="s">
-        <v>949</v>
+        <v>707</v>
       </c>
       <c r="H140" s="3" t="s">
-        <v>42</v>
+        <v>86</v>
       </c>
       <c r="I140" s="3"/>
       <c r="J140" s="3"/>
@@ -15405,13 +15495,13 @@
       <c r="O140" s="4"/>
       <c r="P140" s="10"/>
       <c r="Q140" s="3" t="s">
-        <v>950</v>
+        <v>710</v>
       </c>
       <c r="R140" s="3" t="s">
         <v>52</v>
       </c>
       <c r="S140" s="3" t="s">
-        <v>53</v>
+        <v>91</v>
       </c>
       <c r="T140" s="3">
         <v>1</v>
@@ -15420,17 +15510,17 @@
         <v>54</v>
       </c>
       <c r="V140" s="3" t="s">
-        <v>951</v>
+        <v>955</v>
       </c>
       <c r="W140" s="3" t="s">
-        <v>952</v>
+        <v>857</v>
       </c>
       <c r="X140" s="3" t="s">
-        <v>911</v>
+        <v>956</v>
       </c>
       <c r="Y140" s="3"/>
       <c r="Z140" s="3">
-        <v>0.4</v>
+        <v>1.7</v>
       </c>
       <c r="AA140" s="3"/>
       <c r="AB140" s="3" t="s">
@@ -15459,52 +15549,32 @@
         <v>139</v>
       </c>
       <c r="B141" s="7" t="s">
-        <v>38</v>
+        <v>132</v>
       </c>
       <c r="C141" s="7">
-        <v>2025053506</v>
-      </c>
-      <c r="D141" s="7" t="s">
-        <v>953</v>
-      </c>
-      <c r="E141" s="7" t="s">
-        <v>459</v>
-      </c>
+        <v>2025053457</v>
+      </c>
+      <c r="D141" s="7"/>
+      <c r="E141" s="7"/>
       <c r="F141" s="7">
-        <v>4101</v>
+        <v>3955</v>
       </c>
       <c r="G141" s="7" t="s">
-        <v>363</v>
+        <v>957</v>
       </c>
       <c r="H141" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="I141" s="7" t="s">
-        <v>954</v>
-      </c>
-      <c r="J141" s="7" t="s">
-        <v>274</v>
-      </c>
-      <c r="K141" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="L141" s="7" t="s">
-        <v>244</v>
-      </c>
-      <c r="M141" s="8" t="s">
-        <v>245</v>
-      </c>
-      <c r="N141" s="7">
-        <v>2405</v>
-      </c>
-      <c r="O141" s="8" t="s">
-        <v>541</v>
-      </c>
-      <c r="P141" s="8" t="s">
-        <v>955</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="I141" s="7"/>
+      <c r="J141" s="7"/>
+      <c r="K141" s="7"/>
+      <c r="L141" s="7"/>
+      <c r="M141" s="8"/>
+      <c r="N141" s="7"/>
+      <c r="O141" s="8"/>
+      <c r="P141" s="9"/>
       <c r="Q141" s="7" t="s">
-        <v>364</v>
+        <v>958</v>
       </c>
       <c r="R141" s="7" t="s">
         <v>52</v>
@@ -15519,35 +15589,387 @@
         <v>54</v>
       </c>
       <c r="V141" s="7" t="s">
-        <v>956</v>
+        <v>959</v>
       </c>
       <c r="W141" s="7" t="s">
-        <v>957</v>
+        <v>960</v>
       </c>
       <c r="X141" s="7" t="s">
-        <v>958</v>
-      </c>
-      <c r="Y141" s="7" t="s">
-        <v>959</v>
-      </c>
+        <v>911</v>
+      </c>
+      <c r="Y141" s="7"/>
       <c r="Z141" s="7">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="AA141" s="7"/>
       <c r="AB141" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="AC141" s="8" t="s">
-        <v>960</v>
-      </c>
-      <c r="AD141" s="7"/>
+      <c r="AC141" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="AD141" s="7" t="s">
+        <v>61</v>
+      </c>
       <c r="AE141" s="7"/>
       <c r="AF141" s="7"/>
       <c r="AG141" s="7"/>
       <c r="AH141" s="7"/>
       <c r="AI141" s="7"/>
-      <c r="AJ141" s="7"/>
+      <c r="AJ141" s="7" t="s">
+        <v>61</v>
+      </c>
       <c r="AK141" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="142" spans="1:37">
+      <c r="A142" s="3">
+        <v>140</v>
+      </c>
+      <c r="B142" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C142" s="3">
+        <v>2025053506</v>
+      </c>
+      <c r="D142" s="3" t="s">
+        <v>961</v>
+      </c>
+      <c r="E142" s="3" t="s">
+        <v>459</v>
+      </c>
+      <c r="F142" s="3">
+        <v>4101</v>
+      </c>
+      <c r="G142" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="H142" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="I142" s="3" t="s">
+        <v>962</v>
+      </c>
+      <c r="J142" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="K142" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L142" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="M142" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="N142" s="3">
+        <v>2405</v>
+      </c>
+      <c r="O142" s="4" t="s">
+        <v>541</v>
+      </c>
+      <c r="P142" s="10" t="s">
+        <v>963</v>
+      </c>
+      <c r="Q142" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="R142" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S142" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T142" s="3">
+        <v>1</v>
+      </c>
+      <c r="U142" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V142" s="3" t="s">
+        <v>964</v>
+      </c>
+      <c r="W142" s="3" t="s">
+        <v>965</v>
+      </c>
+      <c r="X142" s="3" t="s">
+        <v>966</v>
+      </c>
+      <c r="Y142" s="3" t="s">
+        <v>967</v>
+      </c>
+      <c r="Z142" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA142" s="3"/>
+      <c r="AB142" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC142" s="10" t="s">
+        <v>968</v>
+      </c>
+      <c r="AD142" s="3"/>
+      <c r="AE142" s="3"/>
+      <c r="AF142" s="3"/>
+      <c r="AG142" s="3"/>
+      <c r="AH142" s="3"/>
+      <c r="AI142" s="3"/>
+      <c r="AJ142" s="3"/>
+      <c r="AK142" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="143" spans="1:37">
+      <c r="A143" s="7">
+        <v>141</v>
+      </c>
+      <c r="B143" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C143" s="7">
+        <v>2025053519</v>
+      </c>
+      <c r="D143" s="7" t="s">
+        <v>969</v>
+      </c>
+      <c r="E143" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F143" s="7">
+        <v>4834</v>
+      </c>
+      <c r="G143" s="7" t="s">
+        <v>312</v>
+      </c>
+      <c r="H143" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="I143" s="7" t="s">
+        <v>970</v>
+      </c>
+      <c r="J143" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="K143" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="L143" s="7" t="s">
+        <v>696</v>
+      </c>
+      <c r="M143" s="8" t="s">
+        <v>697</v>
+      </c>
+      <c r="N143" s="7" t="s">
+        <v>698</v>
+      </c>
+      <c r="O143" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="P143" s="9" t="s">
+        <v>971</v>
+      </c>
+      <c r="Q143" s="7" t="s">
+        <v>313</v>
+      </c>
+      <c r="R143" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S143" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="T143" s="7">
+        <v>1</v>
+      </c>
+      <c r="U143" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V143" s="7" t="s">
+        <v>972</v>
+      </c>
+      <c r="W143" s="7" t="s">
+        <v>973</v>
+      </c>
+      <c r="X143" s="7" t="s">
+        <v>974</v>
+      </c>
+      <c r="Y143" s="7" t="s">
+        <v>975</v>
+      </c>
+      <c r="Z143" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA143" s="7"/>
+      <c r="AB143" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC143" s="9" t="s">
+        <v>976</v>
+      </c>
+      <c r="AD143" s="7"/>
+      <c r="AE143" s="7"/>
+      <c r="AF143" s="7"/>
+      <c r="AG143" s="7"/>
+      <c r="AH143" s="7"/>
+      <c r="AI143" s="7"/>
+      <c r="AJ143" s="7"/>
+      <c r="AK143" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="144" spans="1:37">
+      <c r="A144" s="3">
+        <v>142</v>
+      </c>
+      <c r="B144" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C144" s="3">
+        <v>2025053596</v>
+      </c>
+      <c r="D144" s="3"/>
+      <c r="E144" s="3"/>
+      <c r="F144" s="3">
+        <v>4057</v>
+      </c>
+      <c r="G144" s="3" t="s">
+        <v>977</v>
+      </c>
+      <c r="H144" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="I144" s="3"/>
+      <c r="J144" s="3"/>
+      <c r="K144" s="3"/>
+      <c r="L144" s="3"/>
+      <c r="M144" s="4"/>
+      <c r="N144" s="3"/>
+      <c r="O144" s="4"/>
+      <c r="P144" s="10"/>
+      <c r="Q144" s="3" t="s">
+        <v>978</v>
+      </c>
+      <c r="R144" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S144" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="T144" s="3">
+        <v>1</v>
+      </c>
+      <c r="U144" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V144" s="3" t="s">
+        <v>979</v>
+      </c>
+      <c r="W144" s="3" t="s">
+        <v>980</v>
+      </c>
+      <c r="X144" s="3" t="s">
+        <v>981</v>
+      </c>
+      <c r="Y144" s="3"/>
+      <c r="Z144" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA144" s="3"/>
+      <c r="AB144" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC144" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="AD144" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE144" s="3"/>
+      <c r="AF144" s="3"/>
+      <c r="AG144" s="3"/>
+      <c r="AH144" s="3"/>
+      <c r="AI144" s="3"/>
+      <c r="AJ144" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK144" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="145" spans="1:37">
+      <c r="A145" s="7">
+        <v>143</v>
+      </c>
+      <c r="B145" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="C145" s="7">
+        <v>2025053606</v>
+      </c>
+      <c r="D145" s="7"/>
+      <c r="E145" s="7"/>
+      <c r="F145" s="7">
+        <v>4057</v>
+      </c>
+      <c r="G145" s="7" t="s">
+        <v>977</v>
+      </c>
+      <c r="H145" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="I145" s="7"/>
+      <c r="J145" s="7"/>
+      <c r="K145" s="7"/>
+      <c r="L145" s="7"/>
+      <c r="M145" s="8"/>
+      <c r="N145" s="7"/>
+      <c r="O145" s="8"/>
+      <c r="P145" s="8"/>
+      <c r="Q145" s="7" t="s">
+        <v>978</v>
+      </c>
+      <c r="R145" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S145" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="T145" s="7">
+        <v>1</v>
+      </c>
+      <c r="U145" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V145" s="7" t="s">
+        <v>982</v>
+      </c>
+      <c r="W145" s="7" t="s">
+        <v>981</v>
+      </c>
+      <c r="X145" s="7" t="s">
+        <v>983</v>
+      </c>
+      <c r="Y145" s="7"/>
+      <c r="Z145" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="AA145" s="7"/>
+      <c r="AB145" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC145" s="8" t="s">
+        <v>784</v>
+      </c>
+      <c r="AD145" s="7"/>
+      <c r="AE145" s="7"/>
+      <c r="AF145" s="7"/>
+      <c r="AG145" s="7"/>
+      <c r="AH145" s="7"/>
+      <c r="AI145" s="7"/>
+      <c r="AJ145" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK145" s="7" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit on 2025/05/29 週四 17:17:20.58
</commit_message>
<xml_diff>
--- a/IM/202505_HL_Maintain_Report.xlsx
+++ b/IM/202505_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$145</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$155</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="984">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202505   (  製表日期:2025-05-28  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1054">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202505   (  製表日期:2025-05-29  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -3033,6 +3033,73 @@
     <t>重接排線手動版本更新 測試正常</t>
   </si>
   <si>
+    <t>1D191114052801</t>
+  </si>
+  <si>
+    <t>D191</t>
+  </si>
+  <si>
+    <t>三重興德店</t>
+  </si>
+  <si>
+    <t>2025-05-28 13:15:35</t>
+  </si>
+  <si>
+    <t>TM2(TCX800)無電源反應，門市已有將線路拔除更換插座再開機仍異常，PING81不通無法VNC...請台芝到店協助確認
+與門市確認5/28已清帳，入帳日5/29已有交易，PS若因更換HD.請跟店長宣達:1.請門市先回報代收會計 2.請確認SC的代收資料是否正確 (須與代收單據逐一核對)</t>
+  </si>
+  <si>
+    <t>THILF0D191</t>
+  </si>
+  <si>
+    <t>2025-05-28 13:18:37</t>
+  </si>
+  <si>
+    <t>2025-05-28 14:58:00</t>
+  </si>
+  <si>
+    <t>2025-05-28 15:28:00</t>
+  </si>
+  <si>
+    <t>2025-05-29 17:18:00</t>
+  </si>
+  <si>
+    <t>取消報修，可正常使用</t>
+  </si>
+  <si>
+    <t>1D194114052801</t>
+  </si>
+  <si>
+    <t>2025-05-28 13:24:25</t>
+  </si>
+  <si>
+    <t>HL27</t>
+  </si>
+  <si>
+    <t>HL-雷射印表機</t>
+  </si>
+  <si>
+    <t>多張吃紙、卡紙</t>
+  </si>
+  <si>
+    <t>門市反應sc雷射印表機(L2715DW)面板顯示卡紙無法列印，已有關機重啟確認無卡紙張仍異常...請台芝到店協助</t>
+  </si>
+  <si>
+    <t>2025-05-28 13:26:52</t>
+  </si>
+  <si>
+    <t>2025-05-28 15:42:00</t>
+  </si>
+  <si>
+    <t>2025-05-28 16:12:00</t>
+  </si>
+  <si>
+    <t>2025-05-29 17:26:00</t>
+  </si>
+  <si>
+    <t>將印表機(8103002219)卡紙取出，目前測試正常</t>
+  </si>
+  <si>
     <t>林口香澄店</t>
   </si>
   <si>
@@ -3052,6 +3119,151 @@
   </si>
   <si>
     <t>2025-05-28 14:10:00</t>
+  </si>
+  <si>
+    <t>1D072114052801</t>
+  </si>
+  <si>
+    <t>2025-05-28 14:36:49</t>
+  </si>
+  <si>
+    <t>門市SC鍵盤無反應，確認鍵盤燈有亮，但打字都沒有反應，已有將SC重啟仍無法排除，線路太多門市告知無法重新拔插線......還請台芝到店協助</t>
+  </si>
+  <si>
+    <t>2025-05-28 14:37:51</t>
+  </si>
+  <si>
+    <t>2025-05-29 12:36:00</t>
+  </si>
+  <si>
+    <t>2025-05-29 13:15:00</t>
+  </si>
+  <si>
+    <t>2025-05-29 18:37:00</t>
+  </si>
+  <si>
+    <t>更換SC鍵盤</t>
+  </si>
+  <si>
+    <t>1D072114052802</t>
+  </si>
+  <si>
+    <t>2025-05-28 14:39:22</t>
+  </si>
+  <si>
+    <t>門市反應SC鍵盤異常，打字都沒有反應，但鍵盤燈有亮，已有將SC重啟仍無法排除，門市人員告知線路太多不知道線路是哪條無法協助重新拔插..........還請台芝到店協助</t>
+  </si>
+  <si>
+    <t>2025-05-28 14:40:40</t>
+  </si>
+  <si>
+    <t>2025-05-29 18:40:00</t>
+  </si>
+  <si>
+    <t>14145114052802</t>
+  </si>
+  <si>
+    <t>板橋僑興店</t>
+  </si>
+  <si>
+    <t>2025-05-28 15:28:06</t>
+  </si>
+  <si>
+    <t>門市反應TM2(TCX800)觸控不良,確認沒有貼廣告文宣或是異物觸碰到螢幕,已有協助執行觸控校正但門市告知操作後仍異常......還請台芝到店協助</t>
+  </si>
+  <si>
+    <t>THILF04145</t>
+  </si>
+  <si>
+    <t>2025-05-28 15:29:13</t>
+  </si>
+  <si>
+    <t>2025-05-29 13:35:00</t>
+  </si>
+  <si>
+    <t>2025-05-29 14:20:00</t>
+  </si>
+  <si>
+    <t>2025-05-29 19:29:00</t>
+  </si>
+  <si>
+    <t>客顯螢幕廣告紙盒接觸螢幕導致卡頓
+調整後測試正常</t>
+  </si>
+  <si>
+    <t>1D072114052803</t>
+  </si>
+  <si>
+    <t>2025-05-28 17:50:26</t>
+  </si>
+  <si>
+    <t>門市反應sc螢幕(LCD)黑屏無畫面，門市已重新拔插後方線路仍異常，ping1通可vnc....須請台芝到店協助</t>
+  </si>
+  <si>
+    <t>2025-05-28 17:51:39</t>
+  </si>
+  <si>
+    <t>2025-05-28 17:51:00</t>
+  </si>
+  <si>
+    <t>2025-05-28 18:21:00</t>
+  </si>
+  <si>
+    <t>2025-05-29 21:51:00</t>
+  </si>
+  <si>
+    <t>1D072114052901</t>
+  </si>
+  <si>
+    <t>2025-05-29 13:13:30</t>
+  </si>
+  <si>
+    <t>台芝到店維修查看sc滑鼠異常會協助更換，需協助派工</t>
+  </si>
+  <si>
+    <t>2025-05-29 13:14:16</t>
+  </si>
+  <si>
+    <t>2025-05-29 13:14:00</t>
+  </si>
+  <si>
+    <t>2025-06-02 17:14:00</t>
+  </si>
+  <si>
+    <t>更換SC滑鼠</t>
+  </si>
+  <si>
+    <t>淡水海天店</t>
+  </si>
+  <si>
+    <t>THILF04541</t>
+  </si>
+  <si>
+    <t>2025-05-29 14:25:42</t>
+  </si>
+  <si>
+    <t>2025-05-29 14:00:00</t>
+  </si>
+  <si>
+    <t>2025-05-29 14:24:00</t>
+  </si>
+  <si>
+    <t>2025-05-29 14:28:27</t>
+  </si>
+  <si>
+    <t>淡水沙崙店</t>
+  </si>
+  <si>
+    <t>THILF04802</t>
+  </si>
+  <si>
+    <t>2025-05-29 16:42:34</t>
+  </si>
+  <si>
+    <t>2025-05-29 15:40:00</t>
+  </si>
+  <si>
+    <t>2025-05-29 16:42:00</t>
   </si>
 </sst>
 </file>
@@ -3465,10 +3677,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK145"/>
+  <dimension ref="A1:AK155"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A145" sqref="A145"/>
+      <selection activeCell="A155" sqref="A155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15822,38 +16034,58 @@
         <v>142</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>132</v>
+        <v>38</v>
       </c>
       <c r="C144" s="3">
-        <v>2025053596</v>
-      </c>
-      <c r="D144" s="3"/>
-      <c r="E144" s="3"/>
-      <c r="F144" s="3">
-        <v>4057</v>
+        <v>2025053589</v>
+      </c>
+      <c r="D144" s="3" t="s">
+        <v>977</v>
+      </c>
+      <c r="E144" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F144" s="3" t="s">
+        <v>978</v>
       </c>
       <c r="G144" s="3" t="s">
-        <v>977</v>
+        <v>979</v>
       </c>
       <c r="H144" s="3" t="s">
-        <v>272</v>
-      </c>
-      <c r="I144" s="3"/>
-      <c r="J144" s="3"/>
-      <c r="K144" s="3"/>
-      <c r="L144" s="3"/>
-      <c r="M144" s="4"/>
-      <c r="N144" s="3"/>
-      <c r="O144" s="4"/>
-      <c r="P144" s="10"/>
+        <v>86</v>
+      </c>
+      <c r="I144" s="3" t="s">
+        <v>980</v>
+      </c>
+      <c r="J144" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K144" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L144" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="M144" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="N144" s="3">
+        <v>2306</v>
+      </c>
+      <c r="O144" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="P144" s="10" t="s">
+        <v>981</v>
+      </c>
       <c r="Q144" s="3" t="s">
-        <v>978</v>
+        <v>982</v>
       </c>
       <c r="R144" s="3" t="s">
         <v>52</v>
       </c>
       <c r="S144" s="3" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="T144" s="3">
         <v>1</v>
@@ -15862,36 +16094,34 @@
         <v>54</v>
       </c>
       <c r="V144" s="3" t="s">
-        <v>979</v>
+        <v>983</v>
       </c>
       <c r="W144" s="3" t="s">
-        <v>980</v>
+        <v>984</v>
       </c>
       <c r="X144" s="3" t="s">
-        <v>981</v>
-      </c>
-      <c r="Y144" s="3"/>
+        <v>985</v>
+      </c>
+      <c r="Y144" s="3" t="s">
+        <v>986</v>
+      </c>
       <c r="Z144" s="3">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AA144" s="3"/>
       <c r="AB144" s="3" t="s">
-        <v>59</v>
+        <v>472</v>
       </c>
       <c r="AC144" s="10" t="s">
-        <v>152</v>
-      </c>
-      <c r="AD144" s="3" t="s">
-        <v>61</v>
-      </c>
+        <v>987</v>
+      </c>
+      <c r="AD144" s="3"/>
       <c r="AE144" s="3"/>
       <c r="AF144" s="3"/>
       <c r="AG144" s="3"/>
       <c r="AH144" s="3"/>
       <c r="AI144" s="3"/>
-      <c r="AJ144" s="3" t="s">
-        <v>61</v>
-      </c>
+      <c r="AJ144" s="3"/>
       <c r="AK144" s="3" t="s">
         <v>61</v>
       </c>
@@ -15901,38 +16131,58 @@
         <v>143</v>
       </c>
       <c r="B145" s="7" t="s">
-        <v>132</v>
+        <v>38</v>
       </c>
       <c r="C145" s="7">
-        <v>2025053606</v>
-      </c>
-      <c r="D145" s="7"/>
-      <c r="E145" s="7"/>
-      <c r="F145" s="7">
-        <v>4057</v>
+        <v>2025053590</v>
+      </c>
+      <c r="D145" s="7" t="s">
+        <v>988</v>
+      </c>
+      <c r="E145" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F145" s="7" t="s">
+        <v>410</v>
       </c>
       <c r="G145" s="7" t="s">
-        <v>977</v>
+        <v>411</v>
       </c>
       <c r="H145" s="7" t="s">
-        <v>272</v>
-      </c>
-      <c r="I145" s="7"/>
-      <c r="J145" s="7"/>
-      <c r="K145" s="7"/>
-      <c r="L145" s="7"/>
-      <c r="M145" s="8"/>
-      <c r="N145" s="7"/>
-      <c r="O145" s="8"/>
-      <c r="P145" s="8"/>
+        <v>86</v>
+      </c>
+      <c r="I145" s="7" t="s">
+        <v>989</v>
+      </c>
+      <c r="J145" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="K145" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L145" s="7" t="s">
+        <v>990</v>
+      </c>
+      <c r="M145" s="8" t="s">
+        <v>991</v>
+      </c>
+      <c r="N145" s="7">
+        <v>2701</v>
+      </c>
+      <c r="O145" s="8" t="s">
+        <v>992</v>
+      </c>
+      <c r="P145" s="9" t="s">
+        <v>993</v>
+      </c>
       <c r="Q145" s="7" t="s">
-        <v>978</v>
+        <v>412</v>
       </c>
       <c r="R145" s="7" t="s">
         <v>52</v>
       </c>
       <c r="S145" s="7" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="T145" s="7">
         <v>1</v>
@@ -15941,24 +16191,26 @@
         <v>54</v>
       </c>
       <c r="V145" s="7" t="s">
-        <v>982</v>
+        <v>994</v>
       </c>
       <c r="W145" s="7" t="s">
-        <v>981</v>
+        <v>995</v>
       </c>
       <c r="X145" s="7" t="s">
-        <v>983</v>
-      </c>
-      <c r="Y145" s="7"/>
+        <v>996</v>
+      </c>
+      <c r="Y145" s="7" t="s">
+        <v>997</v>
+      </c>
       <c r="Z145" s="7">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="AA145" s="7"/>
       <c r="AB145" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="AC145" s="8" t="s">
-        <v>784</v>
+      <c r="AC145" s="9" t="s">
+        <v>998</v>
       </c>
       <c r="AD145" s="7"/>
       <c r="AE145" s="7"/>
@@ -15966,10 +16218,882 @@
       <c r="AG145" s="7"/>
       <c r="AH145" s="7"/>
       <c r="AI145" s="7"/>
-      <c r="AJ145" s="7" t="s">
-        <v>61</v>
-      </c>
+      <c r="AJ145" s="7"/>
       <c r="AK145" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="146" spans="1:37">
+      <c r="A146" s="3">
+        <v>144</v>
+      </c>
+      <c r="B146" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C146" s="3">
+        <v>2025053596</v>
+      </c>
+      <c r="D146" s="3"/>
+      <c r="E146" s="3"/>
+      <c r="F146" s="3">
+        <v>4057</v>
+      </c>
+      <c r="G146" s="3" t="s">
+        <v>999</v>
+      </c>
+      <c r="H146" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="I146" s="3"/>
+      <c r="J146" s="3"/>
+      <c r="K146" s="3"/>
+      <c r="L146" s="3"/>
+      <c r="M146" s="4"/>
+      <c r="N146" s="3"/>
+      <c r="O146" s="4"/>
+      <c r="P146" s="10"/>
+      <c r="Q146" s="3" t="s">
+        <v>1000</v>
+      </c>
+      <c r="R146" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S146" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="T146" s="3">
+        <v>1</v>
+      </c>
+      <c r="U146" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V146" s="3" t="s">
+        <v>1001</v>
+      </c>
+      <c r="W146" s="3" t="s">
+        <v>1002</v>
+      </c>
+      <c r="X146" s="3" t="s">
+        <v>1003</v>
+      </c>
+      <c r="Y146" s="3"/>
+      <c r="Z146" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA146" s="3"/>
+      <c r="AB146" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC146" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="AD146" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE146" s="3"/>
+      <c r="AF146" s="3"/>
+      <c r="AG146" s="3"/>
+      <c r="AH146" s="3"/>
+      <c r="AI146" s="3"/>
+      <c r="AJ146" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK146" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="147" spans="1:37">
+      <c r="A147" s="7">
+        <v>145</v>
+      </c>
+      <c r="B147" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="C147" s="7">
+        <v>2025053606</v>
+      </c>
+      <c r="D147" s="7"/>
+      <c r="E147" s="7"/>
+      <c r="F147" s="7">
+        <v>4057</v>
+      </c>
+      <c r="G147" s="7" t="s">
+        <v>999</v>
+      </c>
+      <c r="H147" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="I147" s="7"/>
+      <c r="J147" s="7"/>
+      <c r="K147" s="7"/>
+      <c r="L147" s="7"/>
+      <c r="M147" s="8"/>
+      <c r="N147" s="7"/>
+      <c r="O147" s="8"/>
+      <c r="P147" s="9"/>
+      <c r="Q147" s="7" t="s">
+        <v>1000</v>
+      </c>
+      <c r="R147" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S147" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="T147" s="7">
+        <v>1</v>
+      </c>
+      <c r="U147" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V147" s="7" t="s">
+        <v>1004</v>
+      </c>
+      <c r="W147" s="7" t="s">
+        <v>1003</v>
+      </c>
+      <c r="X147" s="7" t="s">
+        <v>1005</v>
+      </c>
+      <c r="Y147" s="7"/>
+      <c r="Z147" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="AA147" s="7"/>
+      <c r="AB147" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC147" s="9" t="s">
+        <v>784</v>
+      </c>
+      <c r="AD147" s="7"/>
+      <c r="AE147" s="7"/>
+      <c r="AF147" s="7"/>
+      <c r="AG147" s="7"/>
+      <c r="AH147" s="7"/>
+      <c r="AI147" s="7"/>
+      <c r="AJ147" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK147" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="148" spans="1:37">
+      <c r="A148" s="3">
+        <v>146</v>
+      </c>
+      <c r="B148" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C148" s="3">
+        <v>2025053610</v>
+      </c>
+      <c r="D148" s="3" t="s">
+        <v>1006</v>
+      </c>
+      <c r="E148" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F148" s="3" t="s">
+        <v>867</v>
+      </c>
+      <c r="G148" s="3" t="s">
+        <v>868</v>
+      </c>
+      <c r="H148" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I148" s="3" t="s">
+        <v>1007</v>
+      </c>
+      <c r="J148" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K148" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L148" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="M148" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="N148" s="3">
+        <v>2402</v>
+      </c>
+      <c r="O148" s="4" t="s">
+        <v>931</v>
+      </c>
+      <c r="P148" s="10" t="s">
+        <v>1008</v>
+      </c>
+      <c r="Q148" s="3" t="s">
+        <v>873</v>
+      </c>
+      <c r="R148" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S148" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T148" s="3">
+        <v>1</v>
+      </c>
+      <c r="U148" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V148" s="3" t="s">
+        <v>1009</v>
+      </c>
+      <c r="W148" s="3" t="s">
+        <v>1010</v>
+      </c>
+      <c r="X148" s="3" t="s">
+        <v>1011</v>
+      </c>
+      <c r="Y148" s="3" t="s">
+        <v>1012</v>
+      </c>
+      <c r="Z148" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="AA148" s="3"/>
+      <c r="AB148" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC148" s="10" t="s">
+        <v>1013</v>
+      </c>
+      <c r="AD148" s="3"/>
+      <c r="AE148" s="3"/>
+      <c r="AF148" s="3"/>
+      <c r="AG148" s="3"/>
+      <c r="AH148" s="3"/>
+      <c r="AI148" s="3"/>
+      <c r="AJ148" s="3"/>
+      <c r="AK148" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="149" spans="1:37">
+      <c r="A149" s="7">
+        <v>147</v>
+      </c>
+      <c r="B149" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C149" s="7">
+        <v>2025053611</v>
+      </c>
+      <c r="D149" s="7" t="s">
+        <v>1014</v>
+      </c>
+      <c r="E149" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F149" s="7" t="s">
+        <v>867</v>
+      </c>
+      <c r="G149" s="7" t="s">
+        <v>868</v>
+      </c>
+      <c r="H149" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I149" s="7" t="s">
+        <v>1015</v>
+      </c>
+      <c r="J149" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="K149" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L149" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="M149" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="N149" s="7">
+        <v>2402</v>
+      </c>
+      <c r="O149" s="8" t="s">
+        <v>931</v>
+      </c>
+      <c r="P149" s="9" t="s">
+        <v>1016</v>
+      </c>
+      <c r="Q149" s="7" t="s">
+        <v>873</v>
+      </c>
+      <c r="R149" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S149" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="T149" s="7">
+        <v>1</v>
+      </c>
+      <c r="U149" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V149" s="7" t="s">
+        <v>1017</v>
+      </c>
+      <c r="W149" s="7" t="s">
+        <v>1010</v>
+      </c>
+      <c r="X149" s="7" t="s">
+        <v>1011</v>
+      </c>
+      <c r="Y149" s="7" t="s">
+        <v>1018</v>
+      </c>
+      <c r="Z149" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="AA149" s="7"/>
+      <c r="AB149" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC149" s="9" t="s">
+        <v>1013</v>
+      </c>
+      <c r="AD149" s="7"/>
+      <c r="AE149" s="7"/>
+      <c r="AF149" s="7"/>
+      <c r="AG149" s="7"/>
+      <c r="AH149" s="7"/>
+      <c r="AI149" s="7"/>
+      <c r="AJ149" s="7"/>
+      <c r="AK149" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="150" spans="1:37">
+      <c r="A150" s="3">
+        <v>148</v>
+      </c>
+      <c r="B150" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C150" s="3">
+        <v>2025053621</v>
+      </c>
+      <c r="D150" s="3" t="s">
+        <v>1019</v>
+      </c>
+      <c r="E150" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F150" s="3">
+        <v>4145</v>
+      </c>
+      <c r="G150" s="3" t="s">
+        <v>1020</v>
+      </c>
+      <c r="H150" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I150" s="3" t="s">
+        <v>1021</v>
+      </c>
+      <c r="J150" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K150" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L150" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="M150" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="N150" s="3">
+        <v>2307</v>
+      </c>
+      <c r="O150" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="P150" s="10" t="s">
+        <v>1022</v>
+      </c>
+      <c r="Q150" s="3" t="s">
+        <v>1023</v>
+      </c>
+      <c r="R150" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S150" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T150" s="3">
+        <v>1</v>
+      </c>
+      <c r="U150" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V150" s="3" t="s">
+        <v>1024</v>
+      </c>
+      <c r="W150" s="3" t="s">
+        <v>1025</v>
+      </c>
+      <c r="X150" s="3" t="s">
+        <v>1026</v>
+      </c>
+      <c r="Y150" s="3" t="s">
+        <v>1027</v>
+      </c>
+      <c r="Z150" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="AA150" s="3"/>
+      <c r="AB150" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC150" s="10" t="s">
+        <v>1028</v>
+      </c>
+      <c r="AD150" s="3"/>
+      <c r="AE150" s="3"/>
+      <c r="AF150" s="3"/>
+      <c r="AG150" s="3"/>
+      <c r="AH150" s="3"/>
+      <c r="AI150" s="3"/>
+      <c r="AJ150" s="3"/>
+      <c r="AK150" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="151" spans="1:37">
+      <c r="A151" s="7">
+        <v>149</v>
+      </c>
+      <c r="B151" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C151" s="7">
+        <v>2025053714</v>
+      </c>
+      <c r="D151" s="7" t="s">
+        <v>1029</v>
+      </c>
+      <c r="E151" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F151" s="7" t="s">
+        <v>867</v>
+      </c>
+      <c r="G151" s="7" t="s">
+        <v>868</v>
+      </c>
+      <c r="H151" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I151" s="7" t="s">
+        <v>1030</v>
+      </c>
+      <c r="J151" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="K151" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L151" s="7" t="s">
+        <v>628</v>
+      </c>
+      <c r="M151" s="8" t="s">
+        <v>629</v>
+      </c>
+      <c r="N151" s="7">
+        <v>2501</v>
+      </c>
+      <c r="O151" s="8" t="s">
+        <v>630</v>
+      </c>
+      <c r="P151" s="9" t="s">
+        <v>1031</v>
+      </c>
+      <c r="Q151" s="7" t="s">
+        <v>873</v>
+      </c>
+      <c r="R151" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S151" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="T151" s="7">
+        <v>1</v>
+      </c>
+      <c r="U151" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V151" s="7" t="s">
+        <v>1032</v>
+      </c>
+      <c r="W151" s="7" t="s">
+        <v>1033</v>
+      </c>
+      <c r="X151" s="7" t="s">
+        <v>1034</v>
+      </c>
+      <c r="Y151" s="7" t="s">
+        <v>1035</v>
+      </c>
+      <c r="Z151" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA151" s="7"/>
+      <c r="AB151" s="7" t="s">
+        <v>472</v>
+      </c>
+      <c r="AC151" s="9" t="s">
+        <v>473</v>
+      </c>
+      <c r="AD151" s="7"/>
+      <c r="AE151" s="7"/>
+      <c r="AF151" s="7"/>
+      <c r="AG151" s="7"/>
+      <c r="AH151" s="7"/>
+      <c r="AI151" s="7"/>
+      <c r="AJ151" s="7"/>
+      <c r="AK151" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="152" spans="1:37">
+      <c r="A152" s="3">
+        <v>150</v>
+      </c>
+      <c r="B152" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C152" s="3">
+        <v>2025053757</v>
+      </c>
+      <c r="D152" s="3" t="s">
+        <v>1036</v>
+      </c>
+      <c r="E152" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F152" s="3" t="s">
+        <v>867</v>
+      </c>
+      <c r="G152" s="3" t="s">
+        <v>868</v>
+      </c>
+      <c r="H152" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I152" s="3" t="s">
+        <v>1037</v>
+      </c>
+      <c r="J152" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="K152" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L152" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="M152" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="N152" s="3">
+        <v>2403</v>
+      </c>
+      <c r="O152" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="P152" s="10" t="s">
+        <v>1038</v>
+      </c>
+      <c r="Q152" s="3" t="s">
+        <v>873</v>
+      </c>
+      <c r="R152" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S152" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T152" s="3">
+        <v>1</v>
+      </c>
+      <c r="U152" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V152" s="3" t="s">
+        <v>1039</v>
+      </c>
+      <c r="W152" s="3" t="s">
+        <v>1010</v>
+      </c>
+      <c r="X152" s="3" t="s">
+        <v>1040</v>
+      </c>
+      <c r="Y152" s="3" t="s">
+        <v>1041</v>
+      </c>
+      <c r="Z152" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="AA152" s="3"/>
+      <c r="AB152" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC152" s="10" t="s">
+        <v>1042</v>
+      </c>
+      <c r="AD152" s="3"/>
+      <c r="AE152" s="3"/>
+      <c r="AF152" s="3"/>
+      <c r="AG152" s="3"/>
+      <c r="AH152" s="3"/>
+      <c r="AI152" s="3"/>
+      <c r="AJ152" s="3"/>
+      <c r="AK152" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="153" spans="1:37">
+      <c r="A153" s="7">
+        <v>151</v>
+      </c>
+      <c r="B153" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="C153" s="7">
+        <v>2025053762</v>
+      </c>
+      <c r="D153" s="7"/>
+      <c r="E153" s="7"/>
+      <c r="F153" s="7">
+        <v>4541</v>
+      </c>
+      <c r="G153" s="7" t="s">
+        <v>1043</v>
+      </c>
+      <c r="H153" s="7" t="s">
+        <v>479</v>
+      </c>
+      <c r="I153" s="7"/>
+      <c r="J153" s="7"/>
+      <c r="K153" s="7"/>
+      <c r="L153" s="7"/>
+      <c r="M153" s="8"/>
+      <c r="N153" s="7"/>
+      <c r="O153" s="8"/>
+      <c r="P153" s="9"/>
+      <c r="Q153" s="7" t="s">
+        <v>1044</v>
+      </c>
+      <c r="R153" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S153" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="T153" s="7">
+        <v>1</v>
+      </c>
+      <c r="U153" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V153" s="7" t="s">
+        <v>1045</v>
+      </c>
+      <c r="W153" s="7" t="s">
+        <v>1046</v>
+      </c>
+      <c r="X153" s="7" t="s">
+        <v>1047</v>
+      </c>
+      <c r="Y153" s="7"/>
+      <c r="Z153" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="AA153" s="7"/>
+      <c r="AB153" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC153" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="AD153" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE153" s="7"/>
+      <c r="AF153" s="7"/>
+      <c r="AG153" s="7"/>
+      <c r="AH153" s="7"/>
+      <c r="AI153" s="7"/>
+      <c r="AJ153" s="7"/>
+      <c r="AK153" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="154" spans="1:37">
+      <c r="A154" s="3">
+        <v>152</v>
+      </c>
+      <c r="B154" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C154" s="3">
+        <v>2025053763</v>
+      </c>
+      <c r="D154" s="3"/>
+      <c r="E154" s="3"/>
+      <c r="F154" s="3">
+        <v>4145</v>
+      </c>
+      <c r="G154" s="3" t="s">
+        <v>1020</v>
+      </c>
+      <c r="H154" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I154" s="3"/>
+      <c r="J154" s="3"/>
+      <c r="K154" s="3"/>
+      <c r="L154" s="3"/>
+      <c r="M154" s="4"/>
+      <c r="N154" s="3"/>
+      <c r="O154" s="4"/>
+      <c r="P154" s="10"/>
+      <c r="Q154" s="3" t="s">
+        <v>1023</v>
+      </c>
+      <c r="R154" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S154" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T154" s="3">
+        <v>1</v>
+      </c>
+      <c r="U154" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V154" s="3" t="s">
+        <v>1048</v>
+      </c>
+      <c r="W154" s="3" t="s">
+        <v>1025</v>
+      </c>
+      <c r="X154" s="3" t="s">
+        <v>1026</v>
+      </c>
+      <c r="Y154" s="3"/>
+      <c r="Z154" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="AA154" s="3"/>
+      <c r="AB154" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC154" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="AD154" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE154" s="3"/>
+      <c r="AF154" s="3"/>
+      <c r="AG154" s="3"/>
+      <c r="AH154" s="3"/>
+      <c r="AI154" s="3"/>
+      <c r="AJ154" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK154" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="155" spans="1:37">
+      <c r="A155" s="7">
+        <v>153</v>
+      </c>
+      <c r="B155" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="C155" s="7">
+        <v>2025053777</v>
+      </c>
+      <c r="D155" s="7"/>
+      <c r="E155" s="7"/>
+      <c r="F155" s="7">
+        <v>4802</v>
+      </c>
+      <c r="G155" s="7" t="s">
+        <v>1049</v>
+      </c>
+      <c r="H155" s="7" t="s">
+        <v>479</v>
+      </c>
+      <c r="I155" s="7"/>
+      <c r="J155" s="7"/>
+      <c r="K155" s="7"/>
+      <c r="L155" s="7"/>
+      <c r="M155" s="8"/>
+      <c r="N155" s="7"/>
+      <c r="O155" s="8"/>
+      <c r="P155" s="8"/>
+      <c r="Q155" s="7" t="s">
+        <v>1050</v>
+      </c>
+      <c r="R155" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S155" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="T155" s="7">
+        <v>1</v>
+      </c>
+      <c r="U155" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V155" s="7" t="s">
+        <v>1051</v>
+      </c>
+      <c r="W155" s="7" t="s">
+        <v>1052</v>
+      </c>
+      <c r="X155" s="7" t="s">
+        <v>1053</v>
+      </c>
+      <c r="Y155" s="7"/>
+      <c r="Z155" s="7">
+        <v>1</v>
+      </c>
+      <c r="AA155" s="7"/>
+      <c r="AB155" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC155" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="AD155" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE155" s="7"/>
+      <c r="AF155" s="7"/>
+      <c r="AG155" s="7"/>
+      <c r="AH155" s="7"/>
+      <c r="AI155" s="7"/>
+      <c r="AJ155" s="7"/>
+      <c r="AK155" s="7" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>